<commit_message>
adding the template as an internal data file
</commit_message>
<xml_diff>
--- a/inst/template/template-bison.xlsx
+++ b/inst/template/template-bison.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aylapearson/Applications/poisson/shinybisonpic/inst/app/www/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aylapearson/Code/bisonpictools/inst/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF733B2-97AB-054E-838D-F99DA6930414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894F962C-71EB-414B-ABE9-F3D3E105C80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32480" yWindow="840" windowWidth="28040" windowHeight="17440" xr2:uid="{CBEE4468-5A59-B344-A0B5-6F1F38BE5D82}"/>
+    <workbookView xWindow="-32480" yWindow="840" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{CBEE4468-5A59-B344-A0B5-6F1F38BE5D82}"/>
   </bookViews>
   <sheets>
-    <sheet name="Locations" sheetId="2" r:id="rId1"/>
-    <sheet name="Events" sheetId="1" r:id="rId2"/>
+    <sheet name="location" sheetId="2" r:id="rId1"/>
+    <sheet name="event" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF429F2-298F-B542-81FC-B30A5252E1A9}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView zoomScale="135" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8EEA22-A96D-564A-8B74-E04C99EA5D01}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView zoomScale="161" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update template to allow years outside of 2019
</commit_message>
<xml_diff>
--- a/inst/template/template-bison.xlsx
+++ b/inst/template/template-bison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolehill/Code/bisonpictools/inst/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolehill/Code/poissonconsulting/bisonpictools/inst/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B249B3-527B-BA42-952B-01593E500B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4A97C4-B7B7-4F49-A238-E8FC0922A47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40080" yWindow="2280" windowWidth="31040" windowHeight="17140" activeTab="2" xr2:uid="{CBEE4468-5A59-B344-A0B5-6F1F38BE5D82}"/>
+    <workbookView xWindow="40080" yWindow="2280" windowWidth="31040" windowHeight="17140" activeTab="3" xr2:uid="{CBEE4468-5A59-B344-A0B5-6F1F38BE5D82}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="86">
   <si>
     <t>f1</t>
   </si>
@@ -125,9 +125,6 @@
     <t>c("")</t>
   </si>
   <si>
-    <t>c(2019L, 2050L)</t>
-  </si>
-  <si>
     <t>c(1L, 12L)</t>
   </si>
   <si>
@@ -294,6 +291,12 @@
   </si>
   <si>
     <t>Year of census estimate</t>
+  </si>
+  <si>
+    <t>c(2000L, 2050L)</t>
+  </si>
+  <si>
+    <t>c(0, 5)</t>
   </si>
 </sst>
 </file>
@@ -366,9 +369,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -406,7 +409,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -512,7 +515,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -654,7 +657,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -689,7 +692,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1">
         <v>57.895690000000002</v>
@@ -703,13 +706,13 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
         <v>59</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>60</v>
-      </c>
-      <c r="D3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -720,10 +723,10 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
         <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -742,7 +745,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -755,7 +758,7 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView zoomScale="161" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -786,7 +789,7 @@
         <v>26</v>
       </c>
       <c r="H1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
@@ -833,7 +836,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2">
         <v>2019</v>
@@ -898,64 +901,64 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
         <v>42</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>43</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" t="s">
         <v>44</v>
       </c>
-      <c r="F3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>45</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>46</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>47</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>48</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>49</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>50</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>51</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>52</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>53</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>54</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>55</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>56</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>57</v>
-      </c>
-      <c r="U3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -966,61 +969,61 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>29</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>30</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>31</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>32</v>
       </c>
-      <c r="H4" t="s">
-        <v>33</v>
-      </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -1048,10 +1051,10 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
         <v>38</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1064,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4006FEE1-87CE-9C46-B2BC-EF9023708C0F}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1081,19 +1084,19 @@
         <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="G1" s="2"/>
     </row>
@@ -1122,19 +1125,19 @@
         <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1142,19 +1145,19 @@
         <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1175,7 +1178,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1189,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858881B3-B2D6-1B41-B5CC-AA42D2CA7DA2}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1207,19 +1210,19 @@
         <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1247,19 +1250,19 @@
         <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1267,19 +1270,19 @@
         <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1300,7 +1303,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>